<commit_message>
update work status and database create function
</commit_message>
<xml_diff>
--- a/Working status.xlsx
+++ b/Working status.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>20/12/2015</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t>form add exam/ question/ question type ...</t>
+  </si>
+  <si>
+    <t>blog: flash message</t>
+  </si>
+  <si>
+    <t>update register module</t>
+  </si>
+  <si>
+    <t>redirect module</t>
+  </si>
+  <si>
+    <t>update database model</t>
+  </si>
+  <si>
+    <t>using mysql workbench to design</t>
+  </si>
+  <si>
+    <t>note go và cập nhật tự động khác với view từ data có sẵn</t>
   </si>
 </sst>
 </file>
@@ -131,7 +149,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +171,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,6 +228,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,30 +513,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>42375</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>42522</v>
+      </c>
+      <c r="C1" s="3">
+        <v>42705</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -526,18 +556,21 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="2"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -555,18 +588,21 @@
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -584,14 +620,17 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" s="7"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -609,14 +648,15 @@
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" s="7"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -634,14 +674,15 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" s="7"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -659,8 +700,9 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -682,8 +724,9 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7" s="7"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -705,12 +748,15 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" s="7"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -728,12 +774,15 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -751,8 +800,9 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" s="7"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -774,8 +824,9 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" s="7"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -797,6 +848,12 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>